<commit_message>
Adding the button for downloading the Transavia Input files
</commit_message>
<xml_diff>
--- a/Transavia/Consumption/Input_flow_Chicks.xlsx
+++ b/Transavia/Consumption/Input_flow_Chicks.xlsx
@@ -52,28 +52,28 @@
     <t>Santimbru</t>
   </si>
   <si>
-    <t>19.03.2024F2</t>
+    <t>27.03.2024F2</t>
   </si>
   <si>
-    <t>20.03.2024F2</t>
+    <t>28.03.2024F2</t>
   </si>
   <si>
-    <t>21.03.2024F2</t>
+    <t>29.03.2024F2</t>
   </si>
   <si>
-    <t>22.03.2024F2</t>
+    <t>30.03.2024F2</t>
   </si>
   <si>
-    <t>23.03.2024F2</t>
+    <t>31.03.2024F2</t>
   </si>
   <si>
-    <t>24.03.2024F2</t>
+    <t>01.04.2024F2</t>
   </si>
   <si>
-    <t>25.03.2024F2</t>
+    <t>02.04.2024F2</t>
   </si>
   <si>
-    <t>26.03.2024F2</t>
+    <t>03.04.2024F2</t>
   </si>
 </sst>
 </file>
@@ -475,16 +475,16 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2">
-        <v>45370</v>
+        <v>45378</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -501,16 +501,16 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2">
-        <v>45370</v>
+        <v>45378</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -527,16 +527,16 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D4" s="2">
-        <v>45370</v>
+        <v>45378</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -553,16 +553,16 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2">
-        <v>45370</v>
+        <v>45378</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -579,16 +579,16 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2">
-        <v>45370</v>
+        <v>45378</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -605,16 +605,16 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D7" s="2">
-        <v>45370</v>
+        <v>45378</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -631,16 +631,16 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D8" s="2">
-        <v>45370</v>
+        <v>45378</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -657,16 +657,16 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D9" s="2">
-        <v>45370</v>
+        <v>45378</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -683,16 +683,16 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D10" s="2">
-        <v>45370</v>
+        <v>45378</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -709,16 +709,16 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D11" s="2">
-        <v>45370</v>
+        <v>45378</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -735,16 +735,16 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D12" s="2">
-        <v>45370</v>
+        <v>45379</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -756,21 +756,21 @@
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D13" s="2">
-        <v>45370</v>
+        <v>45379</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -782,21 +782,21 @@
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D14" s="2">
-        <v>45371</v>
+        <v>45379</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -813,16 +813,16 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D15" s="2">
-        <v>45371</v>
+        <v>45379</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -839,16 +839,16 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D16" s="2">
-        <v>45371</v>
+        <v>45379</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -865,16 +865,16 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D17" s="2">
-        <v>45371</v>
+        <v>45379</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -891,16 +891,16 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D18" s="2">
-        <v>45371</v>
+        <v>45379</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -917,16 +917,16 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D19" s="2">
-        <v>45371</v>
+        <v>45379</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -943,16 +943,16 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D20" s="2">
-        <v>45371</v>
+        <v>45379</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -969,16 +969,16 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D21" s="2">
-        <v>45371</v>
+        <v>45379</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -995,16 +995,16 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D22" s="2">
-        <v>45371</v>
+        <v>45379</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1021,16 +1021,16 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D23" s="2">
-        <v>45371</v>
+        <v>45379</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1047,16 +1047,16 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D24" s="2">
-        <v>45371</v>
+        <v>45379</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1073,16 +1073,16 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D25" s="2">
-        <v>45371</v>
+        <v>45379</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -1099,16 +1099,16 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D26" s="2">
-        <v>45371</v>
+        <v>45379</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -1125,16 +1125,16 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D27" s="2">
-        <v>45371</v>
+        <v>45379</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -1151,16 +1151,16 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28">
+        <v>16</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
         <v>14</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <v>8</v>
-      </c>
       <c r="D28" s="2">
-        <v>45371</v>
+        <v>45379</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -1177,16 +1177,16 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D29" s="2">
-        <v>45371</v>
+        <v>45379</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
@@ -1203,16 +1203,16 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D30" s="2">
-        <v>45371</v>
+        <v>45379</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
@@ -1229,16 +1229,16 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C31">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D31" s="2">
-        <v>45371</v>
+        <v>45379</v>
       </c>
       <c r="E31" t="s">
         <v>10</v>
@@ -1255,16 +1255,16 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C32">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D32" s="2">
-        <v>45371</v>
+        <v>45379</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
@@ -1281,16 +1281,16 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D33" s="2">
-        <v>45371</v>
+        <v>45379</v>
       </c>
       <c r="E33" t="s">
         <v>10</v>
@@ -1307,16 +1307,16 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D34" s="2">
-        <v>45371</v>
+        <v>45379</v>
       </c>
       <c r="E34" t="s">
         <v>10</v>
@@ -1333,16 +1333,16 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C35">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D35" s="2">
-        <v>45371</v>
+        <v>45379</v>
       </c>
       <c r="E35" t="s">
         <v>10</v>
@@ -1359,16 +1359,16 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D36" s="2">
-        <v>45371</v>
+        <v>45380</v>
       </c>
       <c r="E36" t="s">
         <v>10</v>
@@ -1380,21 +1380,21 @@
         <v>1</v>
       </c>
       <c r="H36" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C37">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D37" s="2">
-        <v>45371</v>
+        <v>45380</v>
       </c>
       <c r="E37" t="s">
         <v>10</v>
@@ -1406,21 +1406,21 @@
         <v>1</v>
       </c>
       <c r="H37" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B38">
         <v>0</v>
       </c>
       <c r="C38">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D38" s="2">
-        <v>45372</v>
+        <v>45380</v>
       </c>
       <c r="E38" t="s">
         <v>10</v>
@@ -1437,16 +1437,16 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B39">
         <v>0</v>
       </c>
       <c r="C39">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D39" s="2">
-        <v>45372</v>
+        <v>45380</v>
       </c>
       <c r="E39" t="s">
         <v>10</v>
@@ -1463,16 +1463,16 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B40">
         <v>0</v>
       </c>
       <c r="C40">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D40" s="2">
-        <v>45372</v>
+        <v>45380</v>
       </c>
       <c r="E40" t="s">
         <v>10</v>
@@ -1489,16 +1489,16 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B41">
         <v>0</v>
       </c>
       <c r="C41">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D41" s="2">
-        <v>45372</v>
+        <v>45380</v>
       </c>
       <c r="E41" t="s">
         <v>10</v>
@@ -1515,16 +1515,16 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B42">
         <v>0</v>
       </c>
       <c r="C42">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D42" s="2">
-        <v>45372</v>
+        <v>45380</v>
       </c>
       <c r="E42" t="s">
         <v>10</v>
@@ -1541,16 +1541,16 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B43">
         <v>0</v>
       </c>
       <c r="C43">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D43" s="2">
-        <v>45372</v>
+        <v>45380</v>
       </c>
       <c r="E43" t="s">
         <v>10</v>
@@ -1567,16 +1567,16 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B44">
         <v>0</v>
       </c>
       <c r="C44">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D44" s="2">
-        <v>45372</v>
+        <v>45380</v>
       </c>
       <c r="E44" t="s">
         <v>10</v>
@@ -1593,16 +1593,16 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B45">
         <v>0</v>
       </c>
       <c r="C45">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D45" s="2">
-        <v>45372</v>
+        <v>45380</v>
       </c>
       <c r="E45" t="s">
         <v>10</v>
@@ -1619,16 +1619,16 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B46">
         <v>0</v>
       </c>
       <c r="C46">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D46" s="2">
-        <v>45372</v>
+        <v>45380</v>
       </c>
       <c r="E46" t="s">
         <v>10</v>
@@ -1645,16 +1645,16 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B47">
         <v>0</v>
       </c>
       <c r="C47">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D47" s="2">
-        <v>45372</v>
+        <v>45380</v>
       </c>
       <c r="E47" t="s">
         <v>10</v>
@@ -1671,16 +1671,16 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B48">
         <v>0</v>
       </c>
       <c r="C48">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D48" s="2">
-        <v>45372</v>
+        <v>45380</v>
       </c>
       <c r="E48" t="s">
         <v>10</v>
@@ -1697,16 +1697,16 @@
     </row>
     <row r="49" spans="1:8">
       <c r="A49">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B49">
         <v>0</v>
       </c>
       <c r="C49">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D49" s="2">
-        <v>45372</v>
+        <v>45380</v>
       </c>
       <c r="E49" t="s">
         <v>10</v>
@@ -1723,16 +1723,16 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B50">
         <v>0</v>
       </c>
       <c r="C50">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D50" s="2">
-        <v>45372</v>
+        <v>45380</v>
       </c>
       <c r="E50" t="s">
         <v>10</v>
@@ -1749,16 +1749,16 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B51">
         <v>0</v>
       </c>
       <c r="C51">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D51" s="2">
-        <v>45372</v>
+        <v>45380</v>
       </c>
       <c r="E51" t="s">
         <v>10</v>
@@ -1775,16 +1775,16 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B52">
         <v>0</v>
       </c>
       <c r="C52">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D52" s="2">
-        <v>45372</v>
+        <v>45380</v>
       </c>
       <c r="E52" t="s">
         <v>10</v>
@@ -1801,16 +1801,16 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B53">
         <v>0</v>
       </c>
       <c r="C53">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D53" s="2">
-        <v>45372</v>
+        <v>45380</v>
       </c>
       <c r="E53" t="s">
         <v>10</v>
@@ -1827,16 +1827,16 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B54">
         <v>0</v>
       </c>
       <c r="C54">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D54" s="2">
-        <v>45372</v>
+        <v>45380</v>
       </c>
       <c r="E54" t="s">
         <v>10</v>
@@ -1853,16 +1853,16 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B55">
         <v>0</v>
       </c>
       <c r="C55">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D55" s="2">
-        <v>45372</v>
+        <v>45380</v>
       </c>
       <c r="E55" t="s">
         <v>10</v>
@@ -1879,16 +1879,16 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B56">
         <v>0</v>
       </c>
       <c r="C56">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D56" s="2">
-        <v>45372</v>
+        <v>45380</v>
       </c>
       <c r="E56" t="s">
         <v>10</v>
@@ -1905,16 +1905,16 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B57">
         <v>0</v>
       </c>
       <c r="C57">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D57" s="2">
-        <v>45372</v>
+        <v>45380</v>
       </c>
       <c r="E57" t="s">
         <v>10</v>
@@ -1931,16 +1931,16 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B58">
         <v>0</v>
       </c>
       <c r="C58">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D58" s="2">
-        <v>45372</v>
+        <v>45380</v>
       </c>
       <c r="E58" t="s">
         <v>10</v>
@@ -1957,16 +1957,16 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B59">
         <v>0</v>
       </c>
       <c r="C59">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D59" s="2">
-        <v>45372</v>
+        <v>45380</v>
       </c>
       <c r="E59" t="s">
         <v>10</v>
@@ -1983,16 +1983,16 @@
     </row>
     <row r="60" spans="1:8">
       <c r="A60">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B60">
         <v>0</v>
       </c>
       <c r="C60">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D60" s="2">
-        <v>45372</v>
+        <v>45381</v>
       </c>
       <c r="E60" t="s">
         <v>10</v>
@@ -2004,21 +2004,21 @@
         <v>1</v>
       </c>
       <c r="H60" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B61">
         <v>0</v>
       </c>
       <c r="C61">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D61" s="2">
-        <v>45372</v>
+        <v>45381</v>
       </c>
       <c r="E61" t="s">
         <v>10</v>
@@ -2030,21 +2030,21 @@
         <v>1</v>
       </c>
       <c r="H61" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B62">
         <v>0</v>
       </c>
       <c r="C62">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D62" s="2">
-        <v>45373</v>
+        <v>45381</v>
       </c>
       <c r="E62" t="s">
         <v>10</v>
@@ -2061,16 +2061,16 @@
     </row>
     <row r="63" spans="1:8">
       <c r="A63">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B63">
         <v>0</v>
       </c>
       <c r="C63">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D63" s="2">
-        <v>45373</v>
+        <v>45381</v>
       </c>
       <c r="E63" t="s">
         <v>10</v>
@@ -2087,16 +2087,16 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B64">
         <v>0</v>
       </c>
       <c r="C64">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D64" s="2">
-        <v>45373</v>
+        <v>45381</v>
       </c>
       <c r="E64" t="s">
         <v>10</v>
@@ -2113,16 +2113,16 @@
     </row>
     <row r="65" spans="1:8">
       <c r="A65">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B65">
         <v>0</v>
       </c>
       <c r="C65">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D65" s="2">
-        <v>45373</v>
+        <v>45381</v>
       </c>
       <c r="E65" t="s">
         <v>10</v>
@@ -2139,16 +2139,16 @@
     </row>
     <row r="66" spans="1:8">
       <c r="A66">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B66">
         <v>0</v>
       </c>
       <c r="C66">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D66" s="2">
-        <v>45373</v>
+        <v>45381</v>
       </c>
       <c r="E66" t="s">
         <v>10</v>
@@ -2165,16 +2165,16 @@
     </row>
     <row r="67" spans="1:8">
       <c r="A67">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B67">
         <v>0</v>
       </c>
       <c r="C67">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D67" s="2">
-        <v>45373</v>
+        <v>45381</v>
       </c>
       <c r="E67" t="s">
         <v>10</v>
@@ -2191,16 +2191,16 @@
     </row>
     <row r="68" spans="1:8">
       <c r="A68">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B68">
         <v>0</v>
       </c>
       <c r="C68">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D68" s="2">
-        <v>45373</v>
+        <v>45381</v>
       </c>
       <c r="E68" t="s">
         <v>10</v>
@@ -2217,16 +2217,16 @@
     </row>
     <row r="69" spans="1:8">
       <c r="A69">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B69">
         <v>0</v>
       </c>
       <c r="C69">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D69" s="2">
-        <v>45373</v>
+        <v>45381</v>
       </c>
       <c r="E69" t="s">
         <v>10</v>
@@ -2243,16 +2243,16 @@
     </row>
     <row r="70" spans="1:8">
       <c r="A70">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B70">
         <v>0</v>
       </c>
       <c r="C70">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="D70" s="2">
-        <v>45373</v>
+        <v>45381</v>
       </c>
       <c r="E70" t="s">
         <v>10</v>
@@ -2269,16 +2269,16 @@
     </row>
     <row r="71" spans="1:8">
       <c r="A71">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B71">
         <v>0</v>
       </c>
       <c r="C71">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="D71" s="2">
-        <v>45373</v>
+        <v>45381</v>
       </c>
       <c r="E71" t="s">
         <v>10</v>
@@ -2295,16 +2295,16 @@
     </row>
     <row r="72" spans="1:8">
       <c r="A72">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B72">
         <v>0</v>
       </c>
       <c r="C72">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D72" s="2">
-        <v>45373</v>
+        <v>45381</v>
       </c>
       <c r="E72" t="s">
         <v>10</v>
@@ -2321,16 +2321,16 @@
     </row>
     <row r="73" spans="1:8">
       <c r="A73">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B73">
         <v>0</v>
       </c>
       <c r="C73">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="D73" s="2">
-        <v>45373</v>
+        <v>45381</v>
       </c>
       <c r="E73" t="s">
         <v>10</v>
@@ -2347,16 +2347,16 @@
     </row>
     <row r="74" spans="1:8">
       <c r="A74">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B74">
         <v>0</v>
       </c>
       <c r="C74">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D74" s="2">
-        <v>45373</v>
+        <v>45381</v>
       </c>
       <c r="E74" t="s">
         <v>10</v>
@@ -2373,16 +2373,16 @@
     </row>
     <row r="75" spans="1:8">
       <c r="A75">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B75">
         <v>0</v>
       </c>
       <c r="C75">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D75" s="2">
-        <v>45373</v>
+        <v>45381</v>
       </c>
       <c r="E75" t="s">
         <v>10</v>
@@ -2399,16 +2399,16 @@
     </row>
     <row r="76" spans="1:8">
       <c r="A76">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B76">
         <v>0</v>
       </c>
       <c r="C76">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D76" s="2">
-        <v>45373</v>
+        <v>45381</v>
       </c>
       <c r="E76" t="s">
         <v>10</v>
@@ -2425,16 +2425,16 @@
     </row>
     <row r="77" spans="1:8">
       <c r="A77">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B77">
         <v>0</v>
       </c>
       <c r="C77">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D77" s="2">
-        <v>45373</v>
+        <v>45381</v>
       </c>
       <c r="E77" t="s">
         <v>10</v>
@@ -2451,16 +2451,16 @@
     </row>
     <row r="78" spans="1:8">
       <c r="A78">
+        <v>18</v>
+      </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
         <v>16</v>
       </c>
-      <c r="B78">
-        <v>0</v>
-      </c>
-      <c r="C78">
-        <v>6</v>
-      </c>
       <c r="D78" s="2">
-        <v>45373</v>
+        <v>45381</v>
       </c>
       <c r="E78" t="s">
         <v>10</v>
@@ -2477,16 +2477,16 @@
     </row>
     <row r="79" spans="1:8">
       <c r="A79">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B79">
         <v>0</v>
       </c>
       <c r="C79">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D79" s="2">
-        <v>45373</v>
+        <v>45381</v>
       </c>
       <c r="E79" t="s">
         <v>10</v>
@@ -2503,16 +2503,16 @@
     </row>
     <row r="80" spans="1:8">
       <c r="A80">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B80">
         <v>0</v>
       </c>
       <c r="C80">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D80" s="2">
-        <v>45373</v>
+        <v>45381</v>
       </c>
       <c r="E80" t="s">
         <v>10</v>
@@ -2529,16 +2529,16 @@
     </row>
     <row r="81" spans="1:8">
       <c r="A81">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B81">
         <v>0</v>
       </c>
       <c r="C81">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D81" s="2">
-        <v>45373</v>
+        <v>45381</v>
       </c>
       <c r="E81" t="s">
         <v>10</v>
@@ -2555,16 +2555,16 @@
     </row>
     <row r="82" spans="1:8">
       <c r="A82">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B82">
         <v>0</v>
       </c>
       <c r="C82">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D82" s="2">
-        <v>45373</v>
+        <v>45381</v>
       </c>
       <c r="E82" t="s">
         <v>10</v>
@@ -2581,16 +2581,16 @@
     </row>
     <row r="83" spans="1:8">
       <c r="A83">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B83">
         <v>0</v>
       </c>
       <c r="C83">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D83" s="2">
-        <v>45373</v>
+        <v>45381</v>
       </c>
       <c r="E83" t="s">
         <v>10</v>
@@ -2607,16 +2607,16 @@
     </row>
     <row r="84" spans="1:8">
       <c r="A84">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B84">
         <v>0</v>
       </c>
       <c r="C84">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D84" s="2">
-        <v>45373</v>
+        <v>45382</v>
       </c>
       <c r="E84" t="s">
         <v>10</v>
@@ -2628,21 +2628,21 @@
         <v>1</v>
       </c>
       <c r="H84" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="85" spans="1:8">
       <c r="A85">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B85">
         <v>0</v>
       </c>
       <c r="C85">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D85" s="2">
-        <v>45373</v>
+        <v>45382</v>
       </c>
       <c r="E85" t="s">
         <v>10</v>
@@ -2654,21 +2654,21 @@
         <v>1</v>
       </c>
       <c r="H85" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="86" spans="1:8">
       <c r="A86">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B86">
         <v>0</v>
       </c>
       <c r="C86">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D86" s="2">
-        <v>45374</v>
+        <v>45382</v>
       </c>
       <c r="E86" t="s">
         <v>10</v>
@@ -2685,16 +2685,16 @@
     </row>
     <row r="87" spans="1:8">
       <c r="A87">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B87">
         <v>0</v>
       </c>
       <c r="C87">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D87" s="2">
-        <v>45374</v>
+        <v>45382</v>
       </c>
       <c r="E87" t="s">
         <v>10</v>
@@ -2711,16 +2711,16 @@
     </row>
     <row r="88" spans="1:8">
       <c r="A88">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B88">
         <v>0</v>
       </c>
       <c r="C88">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D88" s="2">
-        <v>45374</v>
+        <v>45382</v>
       </c>
       <c r="E88" t="s">
         <v>10</v>
@@ -2737,16 +2737,16 @@
     </row>
     <row r="89" spans="1:8">
       <c r="A89">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B89">
         <v>0</v>
       </c>
       <c r="C89">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D89" s="2">
-        <v>45374</v>
+        <v>45382</v>
       </c>
       <c r="E89" t="s">
         <v>10</v>
@@ -2763,16 +2763,16 @@
     </row>
     <row r="90" spans="1:8">
       <c r="A90">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B90">
         <v>0</v>
       </c>
       <c r="C90">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D90" s="2">
-        <v>45374</v>
+        <v>45382</v>
       </c>
       <c r="E90" t="s">
         <v>10</v>
@@ -2789,16 +2789,16 @@
     </row>
     <row r="91" spans="1:8">
       <c r="A91">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B91">
         <v>0</v>
       </c>
       <c r="C91">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D91" s="2">
-        <v>45374</v>
+        <v>45382</v>
       </c>
       <c r="E91" t="s">
         <v>10</v>
@@ -2815,16 +2815,16 @@
     </row>
     <row r="92" spans="1:8">
       <c r="A92">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B92">
         <v>0</v>
       </c>
       <c r="C92">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D92" s="2">
-        <v>45374</v>
+        <v>45382</v>
       </c>
       <c r="E92" t="s">
         <v>10</v>
@@ -2841,16 +2841,16 @@
     </row>
     <row r="93" spans="1:8">
       <c r="A93">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B93">
         <v>0</v>
       </c>
       <c r="C93">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="D93" s="2">
-        <v>45374</v>
+        <v>45382</v>
       </c>
       <c r="E93" t="s">
         <v>10</v>
@@ -2867,16 +2867,16 @@
     </row>
     <row r="94" spans="1:8">
       <c r="A94">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B94">
         <v>0</v>
       </c>
       <c r="C94">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D94" s="2">
-        <v>45374</v>
+        <v>45382</v>
       </c>
       <c r="E94" t="s">
         <v>10</v>
@@ -2893,16 +2893,16 @@
     </row>
     <row r="95" spans="1:8">
       <c r="A95">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B95">
         <v>0</v>
       </c>
       <c r="C95">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D95" s="2">
-        <v>45374</v>
+        <v>45382</v>
       </c>
       <c r="E95" t="s">
         <v>10</v>
@@ -2919,16 +2919,16 @@
     </row>
     <row r="96" spans="1:8">
       <c r="A96">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B96">
         <v>0</v>
       </c>
       <c r="C96">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D96" s="2">
-        <v>45374</v>
+        <v>45382</v>
       </c>
       <c r="E96" t="s">
         <v>10</v>
@@ -2945,16 +2945,16 @@
     </row>
     <row r="97" spans="1:8">
       <c r="A97">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B97">
         <v>0</v>
       </c>
       <c r="C97">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D97" s="2">
-        <v>45374</v>
+        <v>45382</v>
       </c>
       <c r="E97" t="s">
         <v>10</v>
@@ -2971,16 +2971,16 @@
     </row>
     <row r="98" spans="1:8">
       <c r="A98">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B98">
         <v>0</v>
       </c>
       <c r="C98">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D98" s="2">
-        <v>45374</v>
+        <v>45382</v>
       </c>
       <c r="E98" t="s">
         <v>10</v>
@@ -2997,16 +2997,16 @@
     </row>
     <row r="99" spans="1:8">
       <c r="A99">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B99">
         <v>0</v>
       </c>
       <c r="C99">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D99" s="2">
-        <v>45374</v>
+        <v>45382</v>
       </c>
       <c r="E99" t="s">
         <v>10</v>
@@ -3023,16 +3023,16 @@
     </row>
     <row r="100" spans="1:8">
       <c r="A100">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B100">
         <v>0</v>
       </c>
       <c r="C100">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D100" s="2">
-        <v>45374</v>
+        <v>45382</v>
       </c>
       <c r="E100" t="s">
         <v>10</v>
@@ -3049,16 +3049,16 @@
     </row>
     <row r="101" spans="1:8">
       <c r="A101">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B101">
         <v>0</v>
       </c>
       <c r="C101">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D101" s="2">
-        <v>45374</v>
+        <v>45382</v>
       </c>
       <c r="E101" t="s">
         <v>10</v>
@@ -3075,16 +3075,16 @@
     </row>
     <row r="102" spans="1:8">
       <c r="A102">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B102">
         <v>0</v>
       </c>
       <c r="C102">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D102" s="2">
-        <v>45374</v>
+        <v>45382</v>
       </c>
       <c r="E102" t="s">
         <v>10</v>
@@ -3101,16 +3101,16 @@
     </row>
     <row r="103" spans="1:8">
       <c r="A103">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B103">
         <v>0</v>
       </c>
       <c r="C103">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D103" s="2">
-        <v>45374</v>
+        <v>45382</v>
       </c>
       <c r="E103" t="s">
         <v>10</v>
@@ -3127,16 +3127,16 @@
     </row>
     <row r="104" spans="1:8">
       <c r="A104">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B104">
         <v>0</v>
       </c>
       <c r="C104">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D104" s="2">
-        <v>45374</v>
+        <v>45382</v>
       </c>
       <c r="E104" t="s">
         <v>10</v>
@@ -3153,16 +3153,16 @@
     </row>
     <row r="105" spans="1:8">
       <c r="A105">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B105">
         <v>0</v>
       </c>
       <c r="C105">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D105" s="2">
-        <v>45374</v>
+        <v>45382</v>
       </c>
       <c r="E105" t="s">
         <v>10</v>
@@ -3179,16 +3179,16 @@
     </row>
     <row r="106" spans="1:8">
       <c r="A106">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B106">
         <v>0</v>
       </c>
       <c r="C106">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D106" s="2">
-        <v>45374</v>
+        <v>45382</v>
       </c>
       <c r="E106" t="s">
         <v>10</v>
@@ -3205,16 +3205,16 @@
     </row>
     <row r="107" spans="1:8">
       <c r="A107">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B107">
         <v>0</v>
       </c>
       <c r="C107">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D107" s="2">
-        <v>45374</v>
+        <v>45382</v>
       </c>
       <c r="E107" t="s">
         <v>10</v>
@@ -3231,16 +3231,16 @@
     </row>
     <row r="108" spans="1:8">
       <c r="A108">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B108">
         <v>0</v>
       </c>
       <c r="C108">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D108" s="2">
-        <v>45374</v>
+        <v>45383</v>
       </c>
       <c r="E108" t="s">
         <v>10</v>
@@ -3252,21 +3252,21 @@
         <v>1</v>
       </c>
       <c r="H108" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="109" spans="1:8">
       <c r="A109">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B109">
         <v>0</v>
       </c>
       <c r="C109">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D109" s="2">
-        <v>45374</v>
+        <v>45383</v>
       </c>
       <c r="E109" t="s">
         <v>10</v>
@@ -3278,21 +3278,21 @@
         <v>1</v>
       </c>
       <c r="H109" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="110" spans="1:8">
       <c r="A110">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B110">
         <v>0</v>
       </c>
       <c r="C110">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D110" s="2">
-        <v>45375</v>
+        <v>45383</v>
       </c>
       <c r="E110" t="s">
         <v>10</v>
@@ -3309,16 +3309,16 @@
     </row>
     <row r="111" spans="1:8">
       <c r="A111">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B111">
         <v>0</v>
       </c>
       <c r="C111">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D111" s="2">
-        <v>45375</v>
+        <v>45383</v>
       </c>
       <c r="E111" t="s">
         <v>10</v>
@@ -3335,16 +3335,16 @@
     </row>
     <row r="112" spans="1:8">
       <c r="A112">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B112">
         <v>0</v>
       </c>
       <c r="C112">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D112" s="2">
-        <v>45375</v>
+        <v>45383</v>
       </c>
       <c r="E112" t="s">
         <v>10</v>
@@ -3361,16 +3361,16 @@
     </row>
     <row r="113" spans="1:8">
       <c r="A113">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B113">
         <v>0</v>
       </c>
       <c r="C113">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D113" s="2">
-        <v>45375</v>
+        <v>45383</v>
       </c>
       <c r="E113" t="s">
         <v>10</v>
@@ -3387,16 +3387,16 @@
     </row>
     <row r="114" spans="1:8">
       <c r="A114">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B114">
         <v>0</v>
       </c>
       <c r="C114">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D114" s="2">
-        <v>45375</v>
+        <v>45383</v>
       </c>
       <c r="E114" t="s">
         <v>10</v>
@@ -3413,16 +3413,16 @@
     </row>
     <row r="115" spans="1:8">
       <c r="A115">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B115">
         <v>0</v>
       </c>
       <c r="C115">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D115" s="2">
-        <v>45375</v>
+        <v>45383</v>
       </c>
       <c r="E115" t="s">
         <v>10</v>
@@ -3439,16 +3439,16 @@
     </row>
     <row r="116" spans="1:8">
       <c r="A116">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B116">
         <v>0</v>
       </c>
       <c r="C116">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D116" s="2">
-        <v>45375</v>
+        <v>45383</v>
       </c>
       <c r="E116" t="s">
         <v>10</v>
@@ -3465,16 +3465,16 @@
     </row>
     <row r="117" spans="1:8">
       <c r="A117">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B117">
         <v>0</v>
       </c>
       <c r="C117">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D117" s="2">
-        <v>45375</v>
+        <v>45383</v>
       </c>
       <c r="E117" t="s">
         <v>10</v>
@@ -3491,16 +3491,16 @@
     </row>
     <row r="118" spans="1:8">
       <c r="A118">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B118">
         <v>0</v>
       </c>
       <c r="C118">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D118" s="2">
-        <v>45375</v>
+        <v>45383</v>
       </c>
       <c r="E118" t="s">
         <v>10</v>
@@ -3517,16 +3517,16 @@
     </row>
     <row r="119" spans="1:8">
       <c r="A119">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B119">
         <v>0</v>
       </c>
       <c r="C119">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D119" s="2">
-        <v>45375</v>
+        <v>45383</v>
       </c>
       <c r="E119" t="s">
         <v>10</v>
@@ -3543,16 +3543,16 @@
     </row>
     <row r="120" spans="1:8">
       <c r="A120">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B120">
         <v>0</v>
       </c>
       <c r="C120">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D120" s="2">
-        <v>45375</v>
+        <v>45383</v>
       </c>
       <c r="E120" t="s">
         <v>10</v>
@@ -3569,16 +3569,16 @@
     </row>
     <row r="121" spans="1:8">
       <c r="A121">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B121">
         <v>0</v>
       </c>
       <c r="C121">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D121" s="2">
-        <v>45375</v>
+        <v>45383</v>
       </c>
       <c r="E121" t="s">
         <v>10</v>
@@ -3595,16 +3595,16 @@
     </row>
     <row r="122" spans="1:8">
       <c r="A122">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B122">
         <v>0</v>
       </c>
       <c r="C122">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D122" s="2">
-        <v>45375</v>
+        <v>45383</v>
       </c>
       <c r="E122" t="s">
         <v>10</v>
@@ -3621,16 +3621,16 @@
     </row>
     <row r="123" spans="1:8">
       <c r="A123">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B123">
         <v>0</v>
       </c>
       <c r="C123">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D123" s="2">
-        <v>45375</v>
+        <v>45383</v>
       </c>
       <c r="E123" t="s">
         <v>10</v>
@@ -3647,16 +3647,16 @@
     </row>
     <row r="124" spans="1:8">
       <c r="A124">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B124">
         <v>0</v>
       </c>
       <c r="C124">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D124" s="2">
-        <v>45375</v>
+        <v>45383</v>
       </c>
       <c r="E124" t="s">
         <v>10</v>
@@ -3673,16 +3673,16 @@
     </row>
     <row r="125" spans="1:8">
       <c r="A125">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B125">
         <v>0</v>
       </c>
       <c r="C125">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D125" s="2">
-        <v>45375</v>
+        <v>45383</v>
       </c>
       <c r="E125" t="s">
         <v>10</v>
@@ -3699,16 +3699,16 @@
     </row>
     <row r="126" spans="1:8">
       <c r="A126">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B126">
         <v>0</v>
       </c>
       <c r="C126">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D126" s="2">
-        <v>45375</v>
+        <v>45383</v>
       </c>
       <c r="E126" t="s">
         <v>10</v>
@@ -3725,16 +3725,16 @@
     </row>
     <row r="127" spans="1:8">
       <c r="A127">
+        <v>19</v>
+      </c>
+      <c r="B127">
+        <v>0</v>
+      </c>
+      <c r="C127">
         <v>17</v>
       </c>
-      <c r="B127">
-        <v>0</v>
-      </c>
-      <c r="C127">
-        <v>10</v>
-      </c>
       <c r="D127" s="2">
-        <v>45375</v>
+        <v>45383</v>
       </c>
       <c r="E127" t="s">
         <v>10</v>
@@ -3751,16 +3751,16 @@
     </row>
     <row r="128" spans="1:8">
       <c r="A128">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B128">
         <v>0</v>
       </c>
       <c r="C128">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D128" s="2">
-        <v>45375</v>
+        <v>45383</v>
       </c>
       <c r="E128" t="s">
         <v>10</v>
@@ -3777,16 +3777,16 @@
     </row>
     <row r="129" spans="1:8">
       <c r="A129">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B129">
         <v>0</v>
       </c>
       <c r="C129">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D129" s="2">
-        <v>45375</v>
+        <v>45383</v>
       </c>
       <c r="E129" t="s">
         <v>10</v>
@@ -3803,16 +3803,16 @@
     </row>
     <row r="130" spans="1:8">
       <c r="A130">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B130">
         <v>0</v>
       </c>
       <c r="C130">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D130" s="2">
-        <v>45375</v>
+        <v>45383</v>
       </c>
       <c r="E130" t="s">
         <v>10</v>
@@ -3829,16 +3829,16 @@
     </row>
     <row r="131" spans="1:8">
       <c r="A131">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B131">
         <v>0</v>
       </c>
       <c r="C131">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D131" s="2">
-        <v>45375</v>
+        <v>45383</v>
       </c>
       <c r="E131" t="s">
         <v>10</v>
@@ -3855,16 +3855,16 @@
     </row>
     <row r="132" spans="1:8">
       <c r="A132">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B132">
         <v>0</v>
       </c>
       <c r="C132">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D132" s="2">
-        <v>45375</v>
+        <v>45384</v>
       </c>
       <c r="E132" t="s">
         <v>10</v>
@@ -3876,21 +3876,21 @@
         <v>1</v>
       </c>
       <c r="H132" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="133" spans="1:8">
       <c r="A133">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B133">
         <v>0</v>
       </c>
       <c r="C133">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D133" s="2">
-        <v>45375</v>
+        <v>45384</v>
       </c>
       <c r="E133" t="s">
         <v>10</v>
@@ -3902,21 +3902,21 @@
         <v>1</v>
       </c>
       <c r="H133" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="134" spans="1:8">
       <c r="A134">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B134">
         <v>0</v>
       </c>
       <c r="C134">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D134" s="2">
-        <v>45376</v>
+        <v>45384</v>
       </c>
       <c r="E134" t="s">
         <v>10</v>
@@ -3933,16 +3933,16 @@
     </row>
     <row r="135" spans="1:8">
       <c r="A135">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B135">
         <v>0</v>
       </c>
       <c r="C135">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D135" s="2">
-        <v>45376</v>
+        <v>45384</v>
       </c>
       <c r="E135" t="s">
         <v>10</v>
@@ -3959,16 +3959,16 @@
     </row>
     <row r="136" spans="1:8">
       <c r="A136">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B136">
         <v>0</v>
       </c>
       <c r="C136">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D136" s="2">
-        <v>45376</v>
+        <v>45384</v>
       </c>
       <c r="E136" t="s">
         <v>10</v>
@@ -3985,16 +3985,16 @@
     </row>
     <row r="137" spans="1:8">
       <c r="A137">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B137">
         <v>0</v>
       </c>
       <c r="C137">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D137" s="2">
-        <v>45376</v>
+        <v>45384</v>
       </c>
       <c r="E137" t="s">
         <v>10</v>
@@ -4011,16 +4011,16 @@
     </row>
     <row r="138" spans="1:8">
       <c r="A138">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B138">
         <v>0</v>
       </c>
       <c r="C138">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D138" s="2">
-        <v>45376</v>
+        <v>45384</v>
       </c>
       <c r="E138" t="s">
         <v>10</v>
@@ -4037,16 +4037,16 @@
     </row>
     <row r="139" spans="1:8">
       <c r="A139">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B139">
         <v>0</v>
       </c>
       <c r="C139">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D139" s="2">
-        <v>45376</v>
+        <v>45384</v>
       </c>
       <c r="E139" t="s">
         <v>10</v>
@@ -4063,16 +4063,16 @@
     </row>
     <row r="140" spans="1:8">
       <c r="A140">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B140">
         <v>0</v>
       </c>
       <c r="C140">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D140" s="2">
-        <v>45376</v>
+        <v>45384</v>
       </c>
       <c r="E140" t="s">
         <v>10</v>
@@ -4089,16 +4089,16 @@
     </row>
     <row r="141" spans="1:8">
       <c r="A141">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B141">
         <v>0</v>
       </c>
       <c r="C141">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D141" s="2">
-        <v>45376</v>
+        <v>45384</v>
       </c>
       <c r="E141" t="s">
         <v>10</v>
@@ -4115,16 +4115,16 @@
     </row>
     <row r="142" spans="1:8">
       <c r="A142">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B142">
         <v>0</v>
       </c>
       <c r="C142">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D142" s="2">
-        <v>45376</v>
+        <v>45384</v>
       </c>
       <c r="E142" t="s">
         <v>10</v>
@@ -4141,16 +4141,16 @@
     </row>
     <row r="143" spans="1:8">
       <c r="A143">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B143">
         <v>0</v>
       </c>
       <c r="C143">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D143" s="2">
-        <v>45376</v>
+        <v>45384</v>
       </c>
       <c r="E143" t="s">
         <v>10</v>
@@ -4167,16 +4167,16 @@
     </row>
     <row r="144" spans="1:8">
       <c r="A144">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B144">
         <v>0</v>
       </c>
       <c r="C144">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D144" s="2">
-        <v>45376</v>
+        <v>45384</v>
       </c>
       <c r="E144" t="s">
         <v>10</v>
@@ -4193,16 +4193,16 @@
     </row>
     <row r="145" spans="1:8">
       <c r="A145">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B145">
         <v>0</v>
       </c>
       <c r="C145">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D145" s="2">
-        <v>45376</v>
+        <v>45384</v>
       </c>
       <c r="E145" t="s">
         <v>10</v>
@@ -4219,16 +4219,16 @@
     </row>
     <row r="146" spans="1:8">
       <c r="A146">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B146">
         <v>0</v>
       </c>
       <c r="C146">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D146" s="2">
-        <v>45376</v>
+        <v>45384</v>
       </c>
       <c r="E146" t="s">
         <v>10</v>
@@ -4245,16 +4245,16 @@
     </row>
     <row r="147" spans="1:8">
       <c r="A147">
+        <v>15</v>
+      </c>
+      <c r="B147">
+        <v>0</v>
+      </c>
+      <c r="C147">
         <v>13</v>
       </c>
-      <c r="B147">
-        <v>0</v>
-      </c>
-      <c r="C147">
-        <v>7</v>
-      </c>
       <c r="D147" s="2">
-        <v>45376</v>
+        <v>45384</v>
       </c>
       <c r="E147" t="s">
         <v>10</v>
@@ -4271,16 +4271,16 @@
     </row>
     <row r="148" spans="1:8">
       <c r="A148">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B148">
         <v>0</v>
       </c>
       <c r="C148">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D148" s="2">
-        <v>45376</v>
+        <v>45384</v>
       </c>
       <c r="E148" t="s">
         <v>10</v>
@@ -4297,16 +4297,16 @@
     </row>
     <row r="149" spans="1:8">
       <c r="A149">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B149">
         <v>0</v>
       </c>
       <c r="C149">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D149" s="2">
-        <v>45376</v>
+        <v>45384</v>
       </c>
       <c r="E149" t="s">
         <v>10</v>
@@ -4323,16 +4323,16 @@
     </row>
     <row r="150" spans="1:8">
       <c r="A150">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B150">
         <v>0</v>
       </c>
       <c r="C150">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D150" s="2">
-        <v>45376</v>
+        <v>45384</v>
       </c>
       <c r="E150" t="s">
         <v>10</v>
@@ -4349,16 +4349,16 @@
     </row>
     <row r="151" spans="1:8">
       <c r="A151">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B151">
         <v>0</v>
       </c>
       <c r="C151">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D151" s="2">
-        <v>45376</v>
+        <v>45384</v>
       </c>
       <c r="E151" t="s">
         <v>10</v>
@@ -4375,16 +4375,16 @@
     </row>
     <row r="152" spans="1:8">
       <c r="A152">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B152">
         <v>0</v>
       </c>
       <c r="C152">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D152" s="2">
-        <v>45376</v>
+        <v>45384</v>
       </c>
       <c r="E152" t="s">
         <v>10</v>
@@ -4401,16 +4401,16 @@
     </row>
     <row r="153" spans="1:8">
       <c r="A153">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B153">
         <v>0</v>
       </c>
       <c r="C153">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D153" s="2">
-        <v>45376</v>
+        <v>45384</v>
       </c>
       <c r="E153" t="s">
         <v>10</v>
@@ -4427,16 +4427,16 @@
     </row>
     <row r="154" spans="1:8">
       <c r="A154">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B154">
         <v>0</v>
       </c>
       <c r="C154">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D154" s="2">
-        <v>45376</v>
+        <v>45384</v>
       </c>
       <c r="E154" t="s">
         <v>10</v>
@@ -4453,16 +4453,16 @@
     </row>
     <row r="155" spans="1:8">
       <c r="A155">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B155">
         <v>0</v>
       </c>
       <c r="C155">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D155" s="2">
-        <v>45376</v>
+        <v>45384</v>
       </c>
       <c r="E155" t="s">
         <v>10</v>
@@ -4479,16 +4479,16 @@
     </row>
     <row r="156" spans="1:8">
       <c r="A156">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B156">
         <v>0</v>
       </c>
       <c r="C156">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D156" s="2">
-        <v>45376</v>
+        <v>45385</v>
       </c>
       <c r="E156" t="s">
         <v>10</v>
@@ -4500,21 +4500,21 @@
         <v>1</v>
       </c>
       <c r="H156" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="157" spans="1:8">
       <c r="A157">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B157">
         <v>0</v>
       </c>
       <c r="C157">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D157" s="2">
-        <v>45376</v>
+        <v>45385</v>
       </c>
       <c r="E157" t="s">
         <v>10</v>
@@ -4526,21 +4526,21 @@
         <v>1</v>
       </c>
       <c r="H157" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="158" spans="1:8">
       <c r="A158">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B158">
         <v>0</v>
       </c>
       <c r="C158">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D158" s="2">
-        <v>45377</v>
+        <v>45385</v>
       </c>
       <c r="E158" t="s">
         <v>10</v>
@@ -4557,16 +4557,16 @@
     </row>
     <row r="159" spans="1:8">
       <c r="A159">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B159">
         <v>0</v>
       </c>
       <c r="C159">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D159" s="2">
-        <v>45377</v>
+        <v>45385</v>
       </c>
       <c r="E159" t="s">
         <v>10</v>
@@ -4583,16 +4583,16 @@
     </row>
     <row r="160" spans="1:8">
       <c r="A160">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B160">
         <v>0</v>
       </c>
       <c r="C160">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D160" s="2">
-        <v>45377</v>
+        <v>45385</v>
       </c>
       <c r="E160" t="s">
         <v>10</v>
@@ -4609,16 +4609,16 @@
     </row>
     <row r="161" spans="1:8">
       <c r="A161">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B161">
         <v>0</v>
       </c>
       <c r="C161">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D161" s="2">
-        <v>45377</v>
+        <v>45385</v>
       </c>
       <c r="E161" t="s">
         <v>10</v>
@@ -4635,16 +4635,16 @@
     </row>
     <row r="162" spans="1:8">
       <c r="A162">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B162">
         <v>0</v>
       </c>
       <c r="C162">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D162" s="2">
-        <v>45377</v>
+        <v>45385</v>
       </c>
       <c r="E162" t="s">
         <v>10</v>
@@ -4661,16 +4661,16 @@
     </row>
     <row r="163" spans="1:8">
       <c r="A163">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B163">
         <v>0</v>
       </c>
       <c r="C163">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D163" s="2">
-        <v>45377</v>
+        <v>45385</v>
       </c>
       <c r="E163" t="s">
         <v>10</v>
@@ -4687,16 +4687,16 @@
     </row>
     <row r="164" spans="1:8">
       <c r="A164">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B164">
         <v>0</v>
       </c>
       <c r="C164">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D164" s="2">
-        <v>45377</v>
+        <v>45385</v>
       </c>
       <c r="E164" t="s">
         <v>10</v>
@@ -4713,16 +4713,16 @@
     </row>
     <row r="165" spans="1:8">
       <c r="A165">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B165">
         <v>0</v>
       </c>
       <c r="C165">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D165" s="2">
-        <v>45377</v>
+        <v>45385</v>
       </c>
       <c r="E165" t="s">
         <v>10</v>
@@ -4739,16 +4739,16 @@
     </row>
     <row r="166" spans="1:8">
       <c r="A166">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B166">
         <v>0</v>
       </c>
       <c r="C166">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D166" s="2">
-        <v>45377</v>
+        <v>45385</v>
       </c>
       <c r="E166" t="s">
         <v>10</v>
@@ -4765,16 +4765,16 @@
     </row>
     <row r="167" spans="1:8">
       <c r="A167">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B167">
         <v>0</v>
       </c>
       <c r="C167">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D167" s="2">
-        <v>45377</v>
+        <v>45385</v>
       </c>
       <c r="E167" t="s">
         <v>10</v>
@@ -4791,16 +4791,16 @@
     </row>
     <row r="168" spans="1:8">
       <c r="A168">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B168">
         <v>0</v>
       </c>
       <c r="C168">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D168" s="2">
-        <v>45377</v>
+        <v>45385</v>
       </c>
       <c r="E168" t="s">
         <v>10</v>
@@ -4817,16 +4817,16 @@
     </row>
     <row r="169" spans="1:8">
       <c r="A169">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B169">
         <v>0</v>
       </c>
       <c r="C169">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D169" s="2">
-        <v>45377</v>
+        <v>45385</v>
       </c>
       <c r="E169" t="s">
         <v>10</v>
@@ -4843,16 +4843,16 @@
     </row>
     <row r="170" spans="1:8">
       <c r="A170">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B170">
         <v>0</v>
       </c>
       <c r="C170">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D170" s="2">
-        <v>45377</v>
+        <v>45385</v>
       </c>
       <c r="E170" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Retraining the Solina Production model up to June 2024
</commit_message>
<xml_diff>
--- a/Transavia/Consumption/Input_flow_Chicks.xlsx
+++ b/Transavia/Consumption/Input_flow_Chicks.xlsx
@@ -52,18 +52,6 @@
     <t>Santimbru</t>
   </si>
   <si>
-    <t>05.08.2024F2</t>
-  </si>
-  <si>
-    <t>06.08.2024F2</t>
-  </si>
-  <si>
-    <t>07.08.2024F2</t>
-  </si>
-  <si>
-    <t>08.08.2024F2</t>
-  </si>
-  <si>
     <t>09.08.2024F2</t>
   </si>
   <si>
@@ -74,6 +62,18 @@
   </si>
   <si>
     <t>12.08.2024F2</t>
+  </si>
+  <si>
+    <t>13.08.2024F2</t>
+  </si>
+  <si>
+    <t>14.08.2024F2</t>
+  </si>
+  <si>
+    <t>15.08.2024F2</t>
+  </si>
+  <si>
+    <t>16.08.2024F2</t>
   </si>
 </sst>
 </file>
@@ -475,16 +475,16 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2">
-        <v>45509</v>
+        <v>45513</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -501,16 +501,16 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D3" s="2">
-        <v>45509</v>
+        <v>45513</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -527,16 +527,16 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D4" s="2">
-        <v>45509</v>
+        <v>45513</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -553,16 +553,16 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D5" s="2">
-        <v>45509</v>
+        <v>45513</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -579,16 +579,16 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D6" s="2">
-        <v>45509</v>
+        <v>45513</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -605,16 +605,16 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D7" s="2">
-        <v>45509</v>
+        <v>45513</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -631,16 +631,16 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D8" s="2">
-        <v>45509</v>
+        <v>45513</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -657,16 +657,16 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D9" s="2">
-        <v>45510</v>
+        <v>45513</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -678,21 +678,21 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D10" s="2">
-        <v>45510</v>
+        <v>45513</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -704,21 +704,21 @@
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D11" s="2">
-        <v>45510</v>
+        <v>45513</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -730,21 +730,21 @@
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D12" s="2">
-        <v>45510</v>
+        <v>45513</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -756,21 +756,21 @@
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D13" s="2">
-        <v>45510</v>
+        <v>45514</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -787,16 +787,16 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="C14">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D14" s="2">
-        <v>45510</v>
+        <v>45514</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -813,16 +813,16 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
       <c r="C15">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D15" s="2">
-        <v>45510</v>
+        <v>45514</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -839,16 +839,16 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="C16">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D16" s="2">
-        <v>45510</v>
+        <v>45514</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -865,16 +865,16 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B17">
         <v>0</v>
       </c>
       <c r="C17">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D17" s="2">
-        <v>45510</v>
+        <v>45514</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -891,7 +891,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -900,7 +900,7 @@
         <v>16</v>
       </c>
       <c r="D18" s="2">
-        <v>45510</v>
+        <v>45514</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -917,16 +917,16 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="C19">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" s="2">
-        <v>45510</v>
+        <v>45514</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -943,16 +943,16 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
       <c r="C20">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D20" s="2">
-        <v>45510</v>
+        <v>45514</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -969,16 +969,16 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" s="2">
-        <v>45510</v>
+        <v>45514</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -995,7 +995,7 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -1004,7 +1004,7 @@
         <v>18</v>
       </c>
       <c r="D22" s="2">
-        <v>45510</v>
+        <v>45514</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1021,16 +1021,16 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
       <c r="C23">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D23" s="2">
-        <v>45510</v>
+        <v>45514</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1047,16 +1047,16 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
       <c r="C24">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D24" s="2">
-        <v>45510</v>
+        <v>45514</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1073,16 +1073,16 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B25">
         <v>0</v>
       </c>
       <c r="C25">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D25" s="2">
-        <v>45510</v>
+        <v>45514</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -1099,16 +1099,16 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
       <c r="C26">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D26" s="2">
-        <v>45510</v>
+        <v>45514</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -1125,16 +1125,16 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
       <c r="C27">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D27" s="2">
-        <v>45510</v>
+        <v>45514</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -1151,16 +1151,16 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B28">
         <v>0</v>
       </c>
       <c r="C28">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D28" s="2">
-        <v>45510</v>
+        <v>45514</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -1177,16 +1177,16 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B29">
         <v>0</v>
       </c>
       <c r="C29">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D29" s="2">
-        <v>45510</v>
+        <v>45514</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
@@ -1203,16 +1203,16 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
       <c r="C30">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D30" s="2">
-        <v>45510</v>
+        <v>45514</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
@@ -1229,16 +1229,16 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B31">
         <v>0</v>
       </c>
       <c r="C31">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D31" s="2">
-        <v>45510</v>
+        <v>45514</v>
       </c>
       <c r="E31" t="s">
         <v>10</v>
@@ -1255,16 +1255,16 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B32">
         <v>0</v>
       </c>
       <c r="C32">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D32" s="2">
-        <v>45510</v>
+        <v>45514</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
@@ -1281,16 +1281,16 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B33">
         <v>0</v>
       </c>
       <c r="C33">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D33" s="2">
-        <v>45511</v>
+        <v>45514</v>
       </c>
       <c r="E33" t="s">
         <v>10</v>
@@ -1302,21 +1302,21 @@
         <v>1</v>
       </c>
       <c r="H33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B34">
         <v>0</v>
       </c>
       <c r="C34">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D34" s="2">
-        <v>45511</v>
+        <v>45514</v>
       </c>
       <c r="E34" t="s">
         <v>10</v>
@@ -1328,21 +1328,21 @@
         <v>1</v>
       </c>
       <c r="H34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B35">
         <v>0</v>
       </c>
       <c r="C35">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D35" s="2">
-        <v>45511</v>
+        <v>45514</v>
       </c>
       <c r="E35" t="s">
         <v>10</v>
@@ -1354,47 +1354,47 @@
         <v>1</v>
       </c>
       <c r="H35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B36">
         <v>0</v>
       </c>
       <c r="C36">
+        <v>20</v>
+      </c>
+      <c r="D36" s="2">
+        <v>45514</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36" t="s">
         <v>13</v>
-      </c>
-      <c r="D36" s="2">
-        <v>45511</v>
-      </c>
-      <c r="E36" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" t="s">
-        <v>11</v>
-      </c>
-      <c r="G36">
-        <v>1</v>
-      </c>
-      <c r="H36" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B37">
         <v>0</v>
       </c>
       <c r="C37">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D37" s="2">
-        <v>45511</v>
+        <v>45515</v>
       </c>
       <c r="E37" t="s">
         <v>10</v>
@@ -1411,16 +1411,16 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B38">
         <v>0</v>
       </c>
       <c r="C38">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D38" s="2">
-        <v>45511</v>
+        <v>45515</v>
       </c>
       <c r="E38" t="s">
         <v>10</v>
@@ -1437,16 +1437,16 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B39">
         <v>0</v>
       </c>
       <c r="C39">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D39" s="2">
-        <v>45511</v>
+        <v>45515</v>
       </c>
       <c r="E39" t="s">
         <v>10</v>
@@ -1463,16 +1463,16 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B40">
         <v>0</v>
       </c>
       <c r="C40">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D40" s="2">
-        <v>45511</v>
+        <v>45515</v>
       </c>
       <c r="E40" t="s">
         <v>10</v>
@@ -1489,16 +1489,16 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B41">
         <v>0</v>
       </c>
       <c r="C41">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D41" s="2">
-        <v>45511</v>
+        <v>45515</v>
       </c>
       <c r="E41" t="s">
         <v>10</v>
@@ -1515,16 +1515,16 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B42">
         <v>0</v>
       </c>
       <c r="C42">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D42" s="2">
-        <v>45511</v>
+        <v>45515</v>
       </c>
       <c r="E42" t="s">
         <v>10</v>
@@ -1541,7 +1541,7 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -1550,7 +1550,7 @@
         <v>18</v>
       </c>
       <c r="D43" s="2">
-        <v>45511</v>
+        <v>45515</v>
       </c>
       <c r="E43" t="s">
         <v>10</v>
@@ -1567,16 +1567,16 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B44">
         <v>0</v>
       </c>
       <c r="C44">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D44" s="2">
-        <v>45511</v>
+        <v>45515</v>
       </c>
       <c r="E44" t="s">
         <v>10</v>
@@ -1593,16 +1593,16 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B45">
         <v>0</v>
       </c>
       <c r="C45">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D45" s="2">
-        <v>45511</v>
+        <v>45515</v>
       </c>
       <c r="E45" t="s">
         <v>10</v>
@@ -1619,16 +1619,16 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B46">
         <v>0</v>
       </c>
       <c r="C46">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D46" s="2">
-        <v>45511</v>
+        <v>45515</v>
       </c>
       <c r="E46" t="s">
         <v>10</v>
@@ -1645,16 +1645,16 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B47">
         <v>0</v>
       </c>
       <c r="C47">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D47" s="2">
-        <v>45511</v>
+        <v>45515</v>
       </c>
       <c r="E47" t="s">
         <v>10</v>
@@ -1671,7 +1671,7 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -1680,7 +1680,7 @@
         <v>26</v>
       </c>
       <c r="D48" s="2">
-        <v>45511</v>
+        <v>45515</v>
       </c>
       <c r="E48" t="s">
         <v>10</v>
@@ -1697,16 +1697,16 @@
     </row>
     <row r="49" spans="1:8">
       <c r="A49">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B49">
         <v>0</v>
       </c>
       <c r="C49">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D49" s="2">
-        <v>45511</v>
+        <v>45515</v>
       </c>
       <c r="E49" t="s">
         <v>10</v>
@@ -1723,16 +1723,16 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B50">
         <v>0</v>
       </c>
       <c r="C50">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D50" s="2">
-        <v>45511</v>
+        <v>45515</v>
       </c>
       <c r="E50" t="s">
         <v>10</v>
@@ -1749,16 +1749,16 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B51">
         <v>0</v>
       </c>
       <c r="C51">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D51" s="2">
-        <v>45511</v>
+        <v>45515</v>
       </c>
       <c r="E51" t="s">
         <v>10</v>
@@ -1775,16 +1775,16 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B52">
         <v>0</v>
       </c>
       <c r="C52">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D52" s="2">
-        <v>45511</v>
+        <v>45515</v>
       </c>
       <c r="E52" t="s">
         <v>10</v>
@@ -1801,16 +1801,16 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B53">
         <v>0</v>
       </c>
       <c r="C53">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D53" s="2">
-        <v>45511</v>
+        <v>45515</v>
       </c>
       <c r="E53" t="s">
         <v>10</v>
@@ -1827,16 +1827,16 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B54">
         <v>0</v>
       </c>
       <c r="C54">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D54" s="2">
-        <v>45511</v>
+        <v>45515</v>
       </c>
       <c r="E54" t="s">
         <v>10</v>
@@ -1853,16 +1853,16 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B55">
         <v>0</v>
       </c>
       <c r="C55">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="D55" s="2">
-        <v>45511</v>
+        <v>45515</v>
       </c>
       <c r="E55" t="s">
         <v>10</v>
@@ -1879,16 +1879,16 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B56">
         <v>0</v>
       </c>
       <c r="C56">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D56" s="2">
-        <v>45511</v>
+        <v>45515</v>
       </c>
       <c r="E56" t="s">
         <v>10</v>
@@ -1905,16 +1905,16 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B57">
         <v>0</v>
       </c>
       <c r="C57">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D57" s="2">
-        <v>45512</v>
+        <v>45515</v>
       </c>
       <c r="E57" t="s">
         <v>10</v>
@@ -1926,21 +1926,21 @@
         <v>1</v>
       </c>
       <c r="H57" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B58">
         <v>0</v>
       </c>
       <c r="C58">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D58" s="2">
-        <v>45512</v>
+        <v>45515</v>
       </c>
       <c r="E58" t="s">
         <v>10</v>
@@ -1952,21 +1952,21 @@
         <v>1</v>
       </c>
       <c r="H58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B59">
         <v>0</v>
       </c>
       <c r="C59">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D59" s="2">
-        <v>45512</v>
+        <v>45515</v>
       </c>
       <c r="E59" t="s">
         <v>10</v>
@@ -1978,21 +1978,21 @@
         <v>1</v>
       </c>
       <c r="H59" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B60">
         <v>0</v>
       </c>
       <c r="C60">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D60" s="2">
-        <v>45512</v>
+        <v>45515</v>
       </c>
       <c r="E60" t="s">
         <v>10</v>
@@ -2004,21 +2004,21 @@
         <v>1</v>
       </c>
       <c r="H60" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B61">
         <v>0</v>
       </c>
       <c r="C61">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D61" s="2">
-        <v>45512</v>
+        <v>45516</v>
       </c>
       <c r="E61" t="s">
         <v>10</v>
@@ -2035,16 +2035,16 @@
     </row>
     <row r="62" spans="1:8">
       <c r="A62">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B62">
         <v>0</v>
       </c>
       <c r="C62">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D62" s="2">
-        <v>45512</v>
+        <v>45516</v>
       </c>
       <c r="E62" t="s">
         <v>10</v>
@@ -2061,16 +2061,16 @@
     </row>
     <row r="63" spans="1:8">
       <c r="A63">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B63">
         <v>0</v>
       </c>
       <c r="C63">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D63" s="2">
-        <v>45512</v>
+        <v>45516</v>
       </c>
       <c r="E63" t="s">
         <v>10</v>
@@ -2087,16 +2087,16 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B64">
         <v>0</v>
       </c>
       <c r="C64">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D64" s="2">
-        <v>45512</v>
+        <v>45516</v>
       </c>
       <c r="E64" t="s">
         <v>10</v>
@@ -2113,16 +2113,16 @@
     </row>
     <row r="65" spans="1:8">
       <c r="A65">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B65">
         <v>0</v>
       </c>
       <c r="C65">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D65" s="2">
-        <v>45512</v>
+        <v>45516</v>
       </c>
       <c r="E65" t="s">
         <v>10</v>
@@ -2139,7 +2139,7 @@
     </row>
     <row r="66" spans="1:8">
       <c r="A66">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -2148,7 +2148,7 @@
         <v>20</v>
       </c>
       <c r="D66" s="2">
-        <v>45512</v>
+        <v>45516</v>
       </c>
       <c r="E66" t="s">
         <v>10</v>
@@ -2165,16 +2165,16 @@
     </row>
     <row r="67" spans="1:8">
       <c r="A67">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B67">
         <v>0</v>
       </c>
       <c r="C67">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D67" s="2">
-        <v>45512</v>
+        <v>45516</v>
       </c>
       <c r="E67" t="s">
         <v>10</v>
@@ -2191,16 +2191,16 @@
     </row>
     <row r="68" spans="1:8">
       <c r="A68">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B68">
         <v>0</v>
       </c>
       <c r="C68">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D68" s="2">
-        <v>45512</v>
+        <v>45516</v>
       </c>
       <c r="E68" t="s">
         <v>10</v>
@@ -2217,16 +2217,16 @@
     </row>
     <row r="69" spans="1:8">
       <c r="A69">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B69">
         <v>0</v>
       </c>
       <c r="C69">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D69" s="2">
-        <v>45512</v>
+        <v>45516</v>
       </c>
       <c r="E69" t="s">
         <v>10</v>
@@ -2243,16 +2243,16 @@
     </row>
     <row r="70" spans="1:8">
       <c r="A70">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B70">
         <v>0</v>
       </c>
       <c r="C70">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D70" s="2">
-        <v>45512</v>
+        <v>45516</v>
       </c>
       <c r="E70" t="s">
         <v>10</v>
@@ -2269,16 +2269,16 @@
     </row>
     <row r="71" spans="1:8">
       <c r="A71">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B71">
         <v>0</v>
       </c>
       <c r="C71">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D71" s="2">
-        <v>45512</v>
+        <v>45516</v>
       </c>
       <c r="E71" t="s">
         <v>10</v>
@@ -2295,16 +2295,16 @@
     </row>
     <row r="72" spans="1:8">
       <c r="A72">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B72">
         <v>0</v>
       </c>
       <c r="C72">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D72" s="2">
-        <v>45512</v>
+        <v>45516</v>
       </c>
       <c r="E72" t="s">
         <v>10</v>
@@ -2321,16 +2321,16 @@
     </row>
     <row r="73" spans="1:8">
       <c r="A73">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B73">
         <v>0</v>
       </c>
       <c r="C73">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D73" s="2">
-        <v>45512</v>
+        <v>45516</v>
       </c>
       <c r="E73" t="s">
         <v>10</v>
@@ -2347,16 +2347,16 @@
     </row>
     <row r="74" spans="1:8">
       <c r="A74">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B74">
         <v>0</v>
       </c>
       <c r="C74">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D74" s="2">
-        <v>45512</v>
+        <v>45516</v>
       </c>
       <c r="E74" t="s">
         <v>10</v>
@@ -2373,16 +2373,16 @@
     </row>
     <row r="75" spans="1:8">
       <c r="A75">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B75">
         <v>0</v>
       </c>
       <c r="C75">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D75" s="2">
-        <v>45512</v>
+        <v>45516</v>
       </c>
       <c r="E75" t="s">
         <v>10</v>
@@ -2399,16 +2399,16 @@
     </row>
     <row r="76" spans="1:8">
       <c r="A76">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B76">
         <v>0</v>
       </c>
       <c r="C76">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D76" s="2">
-        <v>45512</v>
+        <v>45516</v>
       </c>
       <c r="E76" t="s">
         <v>10</v>
@@ -2425,16 +2425,16 @@
     </row>
     <row r="77" spans="1:8">
       <c r="A77">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B77">
         <v>0</v>
       </c>
       <c r="C77">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D77" s="2">
-        <v>45512</v>
+        <v>45516</v>
       </c>
       <c r="E77" t="s">
         <v>10</v>
@@ -2451,16 +2451,16 @@
     </row>
     <row r="78" spans="1:8">
       <c r="A78">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B78">
         <v>0</v>
       </c>
       <c r="C78">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D78" s="2">
-        <v>45512</v>
+        <v>45516</v>
       </c>
       <c r="E78" t="s">
         <v>10</v>
@@ -2477,16 +2477,16 @@
     </row>
     <row r="79" spans="1:8">
       <c r="A79">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B79">
         <v>0</v>
       </c>
       <c r="C79">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="D79" s="2">
-        <v>45512</v>
+        <v>45516</v>
       </c>
       <c r="E79" t="s">
         <v>10</v>
@@ -2503,16 +2503,16 @@
     </row>
     <row r="80" spans="1:8">
       <c r="A80">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B80">
         <v>0</v>
       </c>
       <c r="C80">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D80" s="2">
-        <v>45512</v>
+        <v>45516</v>
       </c>
       <c r="E80" t="s">
         <v>10</v>
@@ -2529,16 +2529,16 @@
     </row>
     <row r="81" spans="1:8">
       <c r="A81">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B81">
         <v>0</v>
       </c>
       <c r="C81">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D81" s="2">
-        <v>45513</v>
+        <v>45516</v>
       </c>
       <c r="E81" t="s">
         <v>10</v>
@@ -2550,21 +2550,21 @@
         <v>1</v>
       </c>
       <c r="H81" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="82" spans="1:8">
       <c r="A82">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B82">
         <v>0</v>
       </c>
       <c r="C82">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D82" s="2">
-        <v>45513</v>
+        <v>45516</v>
       </c>
       <c r="E82" t="s">
         <v>10</v>
@@ -2576,21 +2576,21 @@
         <v>1</v>
       </c>
       <c r="H82" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="83" spans="1:8">
       <c r="A83">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B83">
         <v>0</v>
       </c>
       <c r="C83">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D83" s="2">
-        <v>45513</v>
+        <v>45516</v>
       </c>
       <c r="E83" t="s">
         <v>10</v>
@@ -2602,21 +2602,21 @@
         <v>1</v>
       </c>
       <c r="H83" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="84" spans="1:8">
       <c r="A84">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B84">
         <v>0</v>
       </c>
       <c r="C84">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D84" s="2">
-        <v>45513</v>
+        <v>45516</v>
       </c>
       <c r="E84" t="s">
         <v>10</v>
@@ -2628,21 +2628,21 @@
         <v>1</v>
       </c>
       <c r="H84" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="85" spans="1:8">
       <c r="A85">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B85">
         <v>0</v>
       </c>
       <c r="C85">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D85" s="2">
-        <v>45513</v>
+        <v>45517</v>
       </c>
       <c r="E85" t="s">
         <v>10</v>
@@ -2659,16 +2659,16 @@
     </row>
     <row r="86" spans="1:8">
       <c r="A86">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B86">
         <v>0</v>
       </c>
       <c r="C86">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D86" s="2">
-        <v>45513</v>
+        <v>45517</v>
       </c>
       <c r="E86" t="s">
         <v>10</v>
@@ -2685,16 +2685,16 @@
     </row>
     <row r="87" spans="1:8">
       <c r="A87">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B87">
         <v>0</v>
       </c>
       <c r="C87">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D87" s="2">
-        <v>45513</v>
+        <v>45517</v>
       </c>
       <c r="E87" t="s">
         <v>10</v>
@@ -2711,16 +2711,16 @@
     </row>
     <row r="88" spans="1:8">
       <c r="A88">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B88">
         <v>0</v>
       </c>
       <c r="C88">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D88" s="2">
-        <v>45513</v>
+        <v>45517</v>
       </c>
       <c r="E88" t="s">
         <v>10</v>
@@ -2737,7 +2737,7 @@
     </row>
     <row r="89" spans="1:8">
       <c r="A89">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -2746,7 +2746,7 @@
         <v>20</v>
       </c>
       <c r="D89" s="2">
-        <v>45513</v>
+        <v>45517</v>
       </c>
       <c r="E89" t="s">
         <v>10</v>
@@ -2763,16 +2763,16 @@
     </row>
     <row r="90" spans="1:8">
       <c r="A90">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B90">
         <v>0</v>
       </c>
       <c r="C90">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D90" s="2">
-        <v>45513</v>
+        <v>45517</v>
       </c>
       <c r="E90" t="s">
         <v>10</v>
@@ -2789,16 +2789,16 @@
     </row>
     <row r="91" spans="1:8">
       <c r="A91">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B91">
         <v>0</v>
       </c>
       <c r="C91">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D91" s="2">
-        <v>45513</v>
+        <v>45517</v>
       </c>
       <c r="E91" t="s">
         <v>10</v>
@@ -2815,16 +2815,16 @@
     </row>
     <row r="92" spans="1:8">
       <c r="A92">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B92">
         <v>0</v>
       </c>
       <c r="C92">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D92" s="2">
-        <v>45513</v>
+        <v>45517</v>
       </c>
       <c r="E92" t="s">
         <v>10</v>
@@ -2841,16 +2841,16 @@
     </row>
     <row r="93" spans="1:8">
       <c r="A93">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B93">
         <v>0</v>
       </c>
       <c r="C93">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D93" s="2">
-        <v>45513</v>
+        <v>45517</v>
       </c>
       <c r="E93" t="s">
         <v>10</v>
@@ -2867,16 +2867,16 @@
     </row>
     <row r="94" spans="1:8">
       <c r="A94">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B94">
         <v>0</v>
       </c>
       <c r="C94">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D94" s="2">
-        <v>45513</v>
+        <v>45517</v>
       </c>
       <c r="E94" t="s">
         <v>10</v>
@@ -2893,16 +2893,16 @@
     </row>
     <row r="95" spans="1:8">
       <c r="A95">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B95">
         <v>0</v>
       </c>
       <c r="C95">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D95" s="2">
-        <v>45513</v>
+        <v>45517</v>
       </c>
       <c r="E95" t="s">
         <v>10</v>
@@ -2919,16 +2919,16 @@
     </row>
     <row r="96" spans="1:8">
       <c r="A96">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B96">
         <v>0</v>
       </c>
       <c r="C96">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D96" s="2">
-        <v>45513</v>
+        <v>45517</v>
       </c>
       <c r="E96" t="s">
         <v>10</v>
@@ -2945,16 +2945,16 @@
     </row>
     <row r="97" spans="1:8">
       <c r="A97">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B97">
         <v>0</v>
       </c>
       <c r="C97">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D97" s="2">
-        <v>45513</v>
+        <v>45517</v>
       </c>
       <c r="E97" t="s">
         <v>10</v>
@@ -2971,16 +2971,16 @@
     </row>
     <row r="98" spans="1:8">
       <c r="A98">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B98">
         <v>0</v>
       </c>
       <c r="C98">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D98" s="2">
-        <v>45513</v>
+        <v>45517</v>
       </c>
       <c r="E98" t="s">
         <v>10</v>
@@ -2997,7 +2997,7 @@
     </row>
     <row r="99" spans="1:8">
       <c r="A99">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -3006,7 +3006,7 @@
         <v>32</v>
       </c>
       <c r="D99" s="2">
-        <v>45513</v>
+        <v>45517</v>
       </c>
       <c r="E99" t="s">
         <v>10</v>
@@ -3023,16 +3023,16 @@
     </row>
     <row r="100" spans="1:8">
       <c r="A100">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B100">
         <v>0</v>
       </c>
       <c r="C100">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D100" s="2">
-        <v>45513</v>
+        <v>45517</v>
       </c>
       <c r="E100" t="s">
         <v>10</v>
@@ -3049,16 +3049,16 @@
     </row>
     <row r="101" spans="1:8">
       <c r="A101">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B101">
         <v>0</v>
       </c>
       <c r="C101">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D101" s="2">
-        <v>45513</v>
+        <v>45517</v>
       </c>
       <c r="E101" t="s">
         <v>10</v>
@@ -3075,16 +3075,16 @@
     </row>
     <row r="102" spans="1:8">
       <c r="A102">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B102">
         <v>0</v>
       </c>
       <c r="C102">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D102" s="2">
-        <v>45513</v>
+        <v>45517</v>
       </c>
       <c r="E102" t="s">
         <v>10</v>
@@ -3101,16 +3101,16 @@
     </row>
     <row r="103" spans="1:8">
       <c r="A103">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B103">
         <v>0</v>
       </c>
       <c r="C103">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D103" s="2">
-        <v>45513</v>
+        <v>45517</v>
       </c>
       <c r="E103" t="s">
         <v>10</v>
@@ -3127,16 +3127,16 @@
     </row>
     <row r="104" spans="1:8">
       <c r="A104">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B104">
         <v>0</v>
       </c>
       <c r="C104">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D104" s="2">
-        <v>45513</v>
+        <v>45517</v>
       </c>
       <c r="E104" t="s">
         <v>10</v>
@@ -3153,16 +3153,16 @@
     </row>
     <row r="105" spans="1:8">
       <c r="A105">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B105">
         <v>0</v>
       </c>
       <c r="C105">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D105" s="2">
-        <v>45514</v>
+        <v>45517</v>
       </c>
       <c r="E105" t="s">
         <v>10</v>
@@ -3174,21 +3174,21 @@
         <v>1</v>
       </c>
       <c r="H105" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="106" spans="1:8">
       <c r="A106">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B106">
         <v>0</v>
       </c>
       <c r="C106">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D106" s="2">
-        <v>45514</v>
+        <v>45517</v>
       </c>
       <c r="E106" t="s">
         <v>10</v>
@@ -3200,21 +3200,21 @@
         <v>1</v>
       </c>
       <c r="H106" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="107" spans="1:8">
       <c r="A107">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B107">
         <v>0</v>
       </c>
       <c r="C107">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D107" s="2">
-        <v>45514</v>
+        <v>45517</v>
       </c>
       <c r="E107" t="s">
         <v>10</v>
@@ -3226,21 +3226,21 @@
         <v>1</v>
       </c>
       <c r="H107" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="108" spans="1:8">
       <c r="A108">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B108">
         <v>0</v>
       </c>
       <c r="C108">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D108" s="2">
-        <v>45514</v>
+        <v>45517</v>
       </c>
       <c r="E108" t="s">
         <v>10</v>
@@ -3252,21 +3252,21 @@
         <v>1</v>
       </c>
       <c r="H108" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="109" spans="1:8">
       <c r="A109">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B109">
         <v>0</v>
       </c>
       <c r="C109">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D109" s="2">
-        <v>45514</v>
+        <v>45518</v>
       </c>
       <c r="E109" t="s">
         <v>10</v>
@@ -3283,16 +3283,16 @@
     </row>
     <row r="110" spans="1:8">
       <c r="A110">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B110">
         <v>0</v>
       </c>
       <c r="C110">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D110" s="2">
-        <v>45514</v>
+        <v>45518</v>
       </c>
       <c r="E110" t="s">
         <v>10</v>
@@ -3309,16 +3309,16 @@
     </row>
     <row r="111" spans="1:8">
       <c r="A111">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B111">
         <v>0</v>
       </c>
       <c r="C111">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D111" s="2">
-        <v>45514</v>
+        <v>45518</v>
       </c>
       <c r="E111" t="s">
         <v>10</v>
@@ -3335,16 +3335,16 @@
     </row>
     <row r="112" spans="1:8">
       <c r="A112">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B112">
         <v>0</v>
       </c>
       <c r="C112">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D112" s="2">
-        <v>45514</v>
+        <v>45518</v>
       </c>
       <c r="E112" t="s">
         <v>10</v>
@@ -3361,16 +3361,16 @@
     </row>
     <row r="113" spans="1:8">
       <c r="A113">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B113">
         <v>0</v>
       </c>
       <c r="C113">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D113" s="2">
-        <v>45514</v>
+        <v>45518</v>
       </c>
       <c r="E113" t="s">
         <v>10</v>
@@ -3387,16 +3387,16 @@
     </row>
     <row r="114" spans="1:8">
       <c r="A114">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B114">
         <v>0</v>
       </c>
       <c r="C114">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D114" s="2">
-        <v>45514</v>
+        <v>45518</v>
       </c>
       <c r="E114" t="s">
         <v>10</v>
@@ -3413,16 +3413,16 @@
     </row>
     <row r="115" spans="1:8">
       <c r="A115">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B115">
         <v>0</v>
       </c>
       <c r="C115">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D115" s="2">
-        <v>45514</v>
+        <v>45518</v>
       </c>
       <c r="E115" t="s">
         <v>10</v>
@@ -3439,16 +3439,16 @@
     </row>
     <row r="116" spans="1:8">
       <c r="A116">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B116">
         <v>0</v>
       </c>
       <c r="C116">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D116" s="2">
-        <v>45514</v>
+        <v>45518</v>
       </c>
       <c r="E116" t="s">
         <v>10</v>
@@ -3465,16 +3465,16 @@
     </row>
     <row r="117" spans="1:8">
       <c r="A117">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B117">
         <v>0</v>
       </c>
       <c r="C117">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D117" s="2">
-        <v>45514</v>
+        <v>45518</v>
       </c>
       <c r="E117" t="s">
         <v>10</v>
@@ -3491,16 +3491,16 @@
     </row>
     <row r="118" spans="1:8">
       <c r="A118">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B118">
         <v>0</v>
       </c>
       <c r="C118">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D118" s="2">
-        <v>45514</v>
+        <v>45518</v>
       </c>
       <c r="E118" t="s">
         <v>10</v>
@@ -3517,16 +3517,16 @@
     </row>
     <row r="119" spans="1:8">
       <c r="A119">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B119">
         <v>0</v>
       </c>
       <c r="C119">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D119" s="2">
-        <v>45514</v>
+        <v>45518</v>
       </c>
       <c r="E119" t="s">
         <v>10</v>
@@ -3543,16 +3543,16 @@
     </row>
     <row r="120" spans="1:8">
       <c r="A120">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B120">
         <v>0</v>
       </c>
       <c r="C120">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D120" s="2">
-        <v>45514</v>
+        <v>45518</v>
       </c>
       <c r="E120" t="s">
         <v>10</v>
@@ -3569,16 +3569,16 @@
     </row>
     <row r="121" spans="1:8">
       <c r="A121">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B121">
         <v>0</v>
       </c>
       <c r="C121">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D121" s="2">
-        <v>45514</v>
+        <v>45518</v>
       </c>
       <c r="E121" t="s">
         <v>10</v>
@@ -3595,16 +3595,16 @@
     </row>
     <row r="122" spans="1:8">
       <c r="A122">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B122">
         <v>0</v>
       </c>
       <c r="C122">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D122" s="2">
-        <v>45514</v>
+        <v>45518</v>
       </c>
       <c r="E122" t="s">
         <v>10</v>
@@ -3621,16 +3621,16 @@
     </row>
     <row r="123" spans="1:8">
       <c r="A123">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B123">
         <v>0</v>
       </c>
       <c r="C123">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D123" s="2">
-        <v>45514</v>
+        <v>45518</v>
       </c>
       <c r="E123" t="s">
         <v>10</v>
@@ -3647,16 +3647,16 @@
     </row>
     <row r="124" spans="1:8">
       <c r="A124">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B124">
         <v>0</v>
       </c>
       <c r="C124">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D124" s="2">
-        <v>45514</v>
+        <v>45518</v>
       </c>
       <c r="E124" t="s">
         <v>10</v>
@@ -3673,16 +3673,16 @@
     </row>
     <row r="125" spans="1:8">
       <c r="A125">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B125">
         <v>0</v>
       </c>
       <c r="C125">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D125" s="2">
-        <v>45514</v>
+        <v>45518</v>
       </c>
       <c r="E125" t="s">
         <v>10</v>
@@ -3699,16 +3699,16 @@
     </row>
     <row r="126" spans="1:8">
       <c r="A126">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B126">
         <v>0</v>
       </c>
       <c r="C126">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D126" s="2">
-        <v>45514</v>
+        <v>45518</v>
       </c>
       <c r="E126" t="s">
         <v>10</v>
@@ -3725,16 +3725,16 @@
     </row>
     <row r="127" spans="1:8">
       <c r="A127">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B127">
         <v>0</v>
       </c>
       <c r="C127">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D127" s="2">
-        <v>45514</v>
+        <v>45518</v>
       </c>
       <c r="E127" t="s">
         <v>10</v>
@@ -3751,16 +3751,16 @@
     </row>
     <row r="128" spans="1:8">
       <c r="A128">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B128">
         <v>0</v>
       </c>
       <c r="C128">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D128" s="2">
-        <v>45514</v>
+        <v>45518</v>
       </c>
       <c r="E128" t="s">
         <v>10</v>
@@ -3777,16 +3777,16 @@
     </row>
     <row r="129" spans="1:8">
       <c r="A129">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B129">
         <v>0</v>
       </c>
       <c r="C129">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D129" s="2">
-        <v>45515</v>
+        <v>45518</v>
       </c>
       <c r="E129" t="s">
         <v>10</v>
@@ -3798,21 +3798,21 @@
         <v>1</v>
       </c>
       <c r="H129" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="130" spans="1:8">
       <c r="A130">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B130">
         <v>0</v>
       </c>
       <c r="C130">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D130" s="2">
-        <v>45515</v>
+        <v>45518</v>
       </c>
       <c r="E130" t="s">
         <v>10</v>
@@ -3824,21 +3824,21 @@
         <v>1</v>
       </c>
       <c r="H130" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="131" spans="1:8">
       <c r="A131">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B131">
         <v>0</v>
       </c>
       <c r="C131">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D131" s="2">
-        <v>45515</v>
+        <v>45518</v>
       </c>
       <c r="E131" t="s">
         <v>10</v>
@@ -3850,21 +3850,21 @@
         <v>1</v>
       </c>
       <c r="H131" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="132" spans="1:8">
       <c r="A132">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B132">
         <v>0</v>
       </c>
       <c r="C132">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D132" s="2">
-        <v>45515</v>
+        <v>45518</v>
       </c>
       <c r="E132" t="s">
         <v>10</v>
@@ -3876,21 +3876,21 @@
         <v>1</v>
       </c>
       <c r="H132" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="133" spans="1:8">
       <c r="A133">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B133">
         <v>0</v>
       </c>
       <c r="C133">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D133" s="2">
-        <v>45515</v>
+        <v>45519</v>
       </c>
       <c r="E133" t="s">
         <v>10</v>
@@ -3907,16 +3907,16 @@
     </row>
     <row r="134" spans="1:8">
       <c r="A134">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B134">
         <v>0</v>
       </c>
       <c r="C134">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D134" s="2">
-        <v>45515</v>
+        <v>45519</v>
       </c>
       <c r="E134" t="s">
         <v>10</v>
@@ -3933,16 +3933,16 @@
     </row>
     <row r="135" spans="1:8">
       <c r="A135">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B135">
         <v>0</v>
       </c>
       <c r="C135">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D135" s="2">
-        <v>45515</v>
+        <v>45519</v>
       </c>
       <c r="E135" t="s">
         <v>10</v>
@@ -3959,16 +3959,16 @@
     </row>
     <row r="136" spans="1:8">
       <c r="A136">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B136">
         <v>0</v>
       </c>
       <c r="C136">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D136" s="2">
-        <v>45515</v>
+        <v>45519</v>
       </c>
       <c r="E136" t="s">
         <v>10</v>
@@ -3985,16 +3985,16 @@
     </row>
     <row r="137" spans="1:8">
       <c r="A137">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B137">
         <v>0</v>
       </c>
       <c r="C137">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D137" s="2">
-        <v>45515</v>
+        <v>45519</v>
       </c>
       <c r="E137" t="s">
         <v>10</v>
@@ -4011,16 +4011,16 @@
     </row>
     <row r="138" spans="1:8">
       <c r="A138">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B138">
         <v>0</v>
       </c>
       <c r="C138">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D138" s="2">
-        <v>45515</v>
+        <v>45519</v>
       </c>
       <c r="E138" t="s">
         <v>10</v>
@@ -4037,16 +4037,16 @@
     </row>
     <row r="139" spans="1:8">
       <c r="A139">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B139">
         <v>0</v>
       </c>
       <c r="C139">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D139" s="2">
-        <v>45515</v>
+        <v>45519</v>
       </c>
       <c r="E139" t="s">
         <v>10</v>
@@ -4063,16 +4063,16 @@
     </row>
     <row r="140" spans="1:8">
       <c r="A140">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B140">
         <v>0</v>
       </c>
       <c r="C140">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D140" s="2">
-        <v>45515</v>
+        <v>45519</v>
       </c>
       <c r="E140" t="s">
         <v>10</v>
@@ -4089,16 +4089,16 @@
     </row>
     <row r="141" spans="1:8">
       <c r="A141">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B141">
         <v>0</v>
       </c>
       <c r="C141">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D141" s="2">
-        <v>45515</v>
+        <v>45519</v>
       </c>
       <c r="E141" t="s">
         <v>10</v>
@@ -4115,16 +4115,16 @@
     </row>
     <row r="142" spans="1:8">
       <c r="A142">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B142">
         <v>0</v>
       </c>
       <c r="C142">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D142" s="2">
-        <v>45515</v>
+        <v>45519</v>
       </c>
       <c r="E142" t="s">
         <v>10</v>
@@ -4141,16 +4141,16 @@
     </row>
     <row r="143" spans="1:8">
       <c r="A143">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B143">
         <v>0</v>
       </c>
       <c r="C143">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D143" s="2">
-        <v>45515</v>
+        <v>45519</v>
       </c>
       <c r="E143" t="s">
         <v>10</v>
@@ -4167,16 +4167,16 @@
     </row>
     <row r="144" spans="1:8">
       <c r="A144">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B144">
         <v>0</v>
       </c>
       <c r="C144">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D144" s="2">
-        <v>45515</v>
+        <v>45519</v>
       </c>
       <c r="E144" t="s">
         <v>10</v>
@@ -4193,16 +4193,16 @@
     </row>
     <row r="145" spans="1:8">
       <c r="A145">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B145">
         <v>0</v>
       </c>
       <c r="C145">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D145" s="2">
-        <v>45515</v>
+        <v>45519</v>
       </c>
       <c r="E145" t="s">
         <v>10</v>
@@ -4219,16 +4219,16 @@
     </row>
     <row r="146" spans="1:8">
       <c r="A146">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B146">
         <v>0</v>
       </c>
       <c r="C146">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D146" s="2">
-        <v>45515</v>
+        <v>45519</v>
       </c>
       <c r="E146" t="s">
         <v>10</v>
@@ -4245,16 +4245,16 @@
     </row>
     <row r="147" spans="1:8">
       <c r="A147">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B147">
         <v>0</v>
       </c>
       <c r="C147">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D147" s="2">
-        <v>45515</v>
+        <v>45519</v>
       </c>
       <c r="E147" t="s">
         <v>10</v>
@@ -4271,16 +4271,16 @@
     </row>
     <row r="148" spans="1:8">
       <c r="A148">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B148">
         <v>0</v>
       </c>
       <c r="C148">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D148" s="2">
-        <v>45515</v>
+        <v>45519</v>
       </c>
       <c r="E148" t="s">
         <v>10</v>
@@ -4297,16 +4297,16 @@
     </row>
     <row r="149" spans="1:8">
       <c r="A149">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B149">
         <v>0</v>
       </c>
       <c r="C149">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D149" s="2">
-        <v>45515</v>
+        <v>45519</v>
       </c>
       <c r="E149" t="s">
         <v>10</v>
@@ -4323,16 +4323,16 @@
     </row>
     <row r="150" spans="1:8">
       <c r="A150">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B150">
         <v>0</v>
       </c>
       <c r="C150">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D150" s="2">
-        <v>45515</v>
+        <v>45519</v>
       </c>
       <c r="E150" t="s">
         <v>10</v>
@@ -4349,16 +4349,16 @@
     </row>
     <row r="151" spans="1:8">
       <c r="A151">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B151">
         <v>0</v>
       </c>
       <c r="C151">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D151" s="2">
-        <v>45515</v>
+        <v>45519</v>
       </c>
       <c r="E151" t="s">
         <v>10</v>
@@ -4375,16 +4375,16 @@
     </row>
     <row r="152" spans="1:8">
       <c r="A152">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B152">
         <v>0</v>
       </c>
       <c r="C152">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D152" s="2">
-        <v>45515</v>
+        <v>45519</v>
       </c>
       <c r="E152" t="s">
         <v>10</v>
@@ -4401,16 +4401,16 @@
     </row>
     <row r="153" spans="1:8">
       <c r="A153">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B153">
         <v>0</v>
       </c>
       <c r="C153">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D153" s="2">
-        <v>45516</v>
+        <v>45519</v>
       </c>
       <c r="E153" t="s">
         <v>10</v>
@@ -4422,21 +4422,21 @@
         <v>1</v>
       </c>
       <c r="H153" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="154" spans="1:8">
       <c r="A154">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B154">
         <v>0</v>
       </c>
       <c r="C154">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D154" s="2">
-        <v>45516</v>
+        <v>45519</v>
       </c>
       <c r="E154" t="s">
         <v>10</v>
@@ -4448,21 +4448,21 @@
         <v>1</v>
       </c>
       <c r="H154" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="155" spans="1:8">
       <c r="A155">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B155">
         <v>0</v>
       </c>
       <c r="C155">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D155" s="2">
-        <v>45516</v>
+        <v>45519</v>
       </c>
       <c r="E155" t="s">
         <v>10</v>
@@ -4474,21 +4474,21 @@
         <v>1</v>
       </c>
       <c r="H155" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="156" spans="1:8">
       <c r="A156">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B156">
         <v>0</v>
       </c>
       <c r="C156">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D156" s="2">
-        <v>45516</v>
+        <v>45519</v>
       </c>
       <c r="E156" t="s">
         <v>10</v>
@@ -4500,21 +4500,21 @@
         <v>1</v>
       </c>
       <c r="H156" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="157" spans="1:8">
       <c r="A157">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B157">
         <v>0</v>
       </c>
       <c r="C157">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D157" s="2">
-        <v>45516</v>
+        <v>45520</v>
       </c>
       <c r="E157" t="s">
         <v>10</v>
@@ -4531,16 +4531,16 @@
     </row>
     <row r="158" spans="1:8">
       <c r="A158">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B158">
         <v>0</v>
       </c>
       <c r="C158">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D158" s="2">
-        <v>45516</v>
+        <v>45520</v>
       </c>
       <c r="E158" t="s">
         <v>10</v>
@@ -4557,16 +4557,16 @@
     </row>
     <row r="159" spans="1:8">
       <c r="A159">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B159">
         <v>0</v>
       </c>
       <c r="C159">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D159" s="2">
-        <v>45516</v>
+        <v>45520</v>
       </c>
       <c r="E159" t="s">
         <v>10</v>
@@ -4583,16 +4583,16 @@
     </row>
     <row r="160" spans="1:8">
       <c r="A160">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B160">
         <v>0</v>
       </c>
       <c r="C160">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D160" s="2">
-        <v>45516</v>
+        <v>45520</v>
       </c>
       <c r="E160" t="s">
         <v>10</v>
@@ -4609,7 +4609,7 @@
     </row>
     <row r="161" spans="1:8">
       <c r="A161">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B161">
         <v>0</v>
@@ -4618,7 +4618,7 @@
         <v>21</v>
       </c>
       <c r="D161" s="2">
-        <v>45516</v>
+        <v>45520</v>
       </c>
       <c r="E161" t="s">
         <v>10</v>
@@ -4635,16 +4635,16 @@
     </row>
     <row r="162" spans="1:8">
       <c r="A162">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B162">
         <v>0</v>
       </c>
       <c r="C162">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D162" s="2">
-        <v>45516</v>
+        <v>45520</v>
       </c>
       <c r="E162" t="s">
         <v>10</v>
@@ -4661,16 +4661,16 @@
     </row>
     <row r="163" spans="1:8">
       <c r="A163">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B163">
         <v>0</v>
       </c>
       <c r="C163">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D163" s="2">
-        <v>45516</v>
+        <v>45520</v>
       </c>
       <c r="E163" t="s">
         <v>10</v>
@@ -4687,16 +4687,16 @@
     </row>
     <row r="164" spans="1:8">
       <c r="A164">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B164">
         <v>0</v>
       </c>
       <c r="C164">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D164" s="2">
-        <v>45516</v>
+        <v>45520</v>
       </c>
       <c r="E164" t="s">
         <v>10</v>
@@ -4713,16 +4713,16 @@
     </row>
     <row r="165" spans="1:8">
       <c r="A165">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B165">
         <v>0</v>
       </c>
       <c r="C165">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D165" s="2">
-        <v>45516</v>
+        <v>45520</v>
       </c>
       <c r="E165" t="s">
         <v>10</v>
@@ -4739,16 +4739,16 @@
     </row>
     <row r="166" spans="1:8">
       <c r="A166">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B166">
         <v>0</v>
       </c>
       <c r="C166">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D166" s="2">
-        <v>45516</v>
+        <v>45520</v>
       </c>
       <c r="E166" t="s">
         <v>10</v>
@@ -4765,16 +4765,16 @@
     </row>
     <row r="167" spans="1:8">
       <c r="A167">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B167">
         <v>0</v>
       </c>
       <c r="C167">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D167" s="2">
-        <v>45516</v>
+        <v>45520</v>
       </c>
       <c r="E167" t="s">
         <v>10</v>
@@ -4791,16 +4791,16 @@
     </row>
     <row r="168" spans="1:8">
       <c r="A168">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B168">
         <v>0</v>
       </c>
       <c r="C168">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D168" s="2">
-        <v>45516</v>
+        <v>45520</v>
       </c>
       <c r="E168" t="s">
         <v>10</v>
@@ -4817,16 +4817,16 @@
     </row>
     <row r="169" spans="1:8">
       <c r="A169">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B169">
         <v>0</v>
       </c>
       <c r="C169">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D169" s="2">
-        <v>45516</v>
+        <v>45520</v>
       </c>
       <c r="E169" t="s">
         <v>10</v>
@@ -4843,16 +4843,16 @@
     </row>
     <row r="170" spans="1:8">
       <c r="A170">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B170">
         <v>0</v>
       </c>
       <c r="C170">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D170" s="2">
-        <v>45516</v>
+        <v>45520</v>
       </c>
       <c r="E170" t="s">
         <v>10</v>

</xml_diff>